<commit_message>
Rimuove file vecchi e aggiorna script con percorsi relativi
</commit_message>
<xml_diff>
--- a/Formazioni/Formazione_Franz.xlsx
+++ b/Formazioni/Formazione_Franz.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,11 +517,11 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>125810</v>
+        <v>141312</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>José Palomino</t>
+          <t>Davide Zappacosta</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -531,7 +531,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>D, C</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -557,16 +557,16 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>85070</v>
+        <v>418579</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Marten De Roon</t>
+          <t>Emil Holm</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Atalanta</t>
+          <t>Bologna</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -597,11 +597,11 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>135890</v>
+        <v>64075</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Hans Hateboer</t>
+          <t>Rafael Tolói</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>D, C</t>
+          <t>D</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -677,11 +677,11 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>432552</v>
+        <v>454908</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Giovanni Bonfanti</t>
+          <t>Isak Hien</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -717,11 +717,11 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>299451</v>
+        <v>84190</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Ademola Lookman</t>
+          <t>Luis Muriel</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -757,11 +757,11 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>343308</v>
+        <v>299451</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Teun Koopmeiners</t>
+          <t>Ademola Lookman</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -771,7 +771,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>D, C</t>
+          <t>C, A</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -797,11 +797,11 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>362556</v>
+        <v>85070</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Éderson</t>
+          <t>Marten De Roon</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -811,7 +811,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D, C</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -837,11 +837,11 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>480468</v>
+        <v>362556</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Leonardo Mendicino</t>
+          <t>Éderson</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -877,11 +877,11 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>84190</v>
+        <v>302650</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Luis Muriel</t>
+          <t>Gianluca Scamacca</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -891,7 +891,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>C, A</t>
+          <t>A</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -917,16 +917,16 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>302650</v>
+        <v>391527</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Gianluca Scamacca</t>
+          <t>El Bilal Touré</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Atalanta</t>
+          <t>Stuttgart</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -953,21 +953,21 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>391527</v>
+        <v>356176</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>El Bilal Touré</t>
+          <t>Michel Adopo</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Atalanta</t>
+          <t>Cagliari</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -982,6 +982,78 @@
       </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
+        <is>
+          <t>Franz</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>432552</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Giovanni Bonfanti</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Atalanta</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Squadra2</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>5-4-1</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Franz</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>125810</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>José Palomino</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Squadra2</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>5-4-1</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
         <is>
           <t>Franz</t>
         </is>

</xml_diff>